<commit_message>
add 1000 player connect id fixed
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\UnderwaterRestaurantGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFB2F5A-9D85-488E-80A4-8B75EEEDEA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B187E5AE-ACF8-4305-ABB5-F63EDE1843F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19665" yWindow="0" windowWidth="18735" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Commands</t>
   </si>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N617"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,6 +590,24 @@
       <c r="F13" t="s">
         <v>23</v>
       </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14" s="1">

</xml_diff>

<commit_message>
Command and server py updates
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\UnderwaterRestaurantGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC10ED-BFC5-424F-9502-B1C788CD53D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839379B7-179E-4AA3-8222-3300D7D51117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19665" yWindow="0" windowWidth="18735" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="18720" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Commands</t>
   </si>
@@ -122,6 +122,12 @@
   <si>
     <t>Economy</t>
   </si>
+  <si>
+    <t>Client-&gt;Server Messages begin with C, Server-&gt;Client Messages Begin with S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Messages are Split with ; </t>
+  </si>
 </sst>
 </file>
 
@@ -195,31 +201,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -505,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N617"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,44 +513,52 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -847,83 +846,82 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>49</v>
       </c>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>52</v>
       </c>
@@ -3696,7 +3694,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B12:B66">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add half of the item system
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\UnderwaterRestaurantGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839379B7-179E-4AA3-8222-3300D7D51117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099CB5CA-F697-4843-A5F4-FA4D953A27C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="18720" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19665" yWindow="0" windowWidth="18735" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Network" sheetId="1" r:id="rId1"/>
+    <sheet name="Items" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>Commands</t>
   </si>
@@ -127,13 +128,103 @@
   </si>
   <si>
     <t xml:space="preserve">Full Messages are Split with ; </t>
+  </si>
+  <si>
+    <t>FROM HERE STATIONS BEGIN</t>
+  </si>
+  <si>
+    <t>Snacks Station</t>
+  </si>
+  <si>
+    <t>destroyItem</t>
+  </si>
+  <si>
+    <t>ItemType</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Coke Bottle</t>
+  </si>
+  <si>
+    <t>State15</t>
+  </si>
+  <si>
+    <t>State14</t>
+  </si>
+  <si>
+    <t>State13</t>
+  </si>
+  <si>
+    <t>State12</t>
+  </si>
+  <si>
+    <t>State11</t>
+  </si>
+  <si>
+    <t>State10</t>
+  </si>
+  <si>
+    <t>State9</t>
+  </si>
+  <si>
+    <t>State8</t>
+  </si>
+  <si>
+    <t>State7</t>
+  </si>
+  <si>
+    <t>State6</t>
+  </si>
+  <si>
+    <t>State5</t>
+  </si>
+  <si>
+    <t>State4</t>
+  </si>
+  <si>
+    <t>State3</t>
+  </si>
+  <si>
+    <t>State2</t>
+  </si>
+  <si>
+    <t>State1</t>
+  </si>
+  <si>
+    <t>State0</t>
+  </si>
+  <si>
+    <t>Open = 1 Closed = 0</t>
+  </si>
+  <si>
+    <t>changeItemState</t>
+  </si>
+  <si>
+    <t>NewState</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Server-&gt;Client</t>
+  </si>
+  <si>
+    <t>Client-&gt;Server</t>
+  </si>
+  <si>
+    <t>X Value*10</t>
+  </si>
+  <si>
+    <t>Y Value*10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,13 +238,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -201,11 +330,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N617"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +656,16 @@
         <v>33</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D8" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -569,7 +714,7 @@
       <c r="C12" s="1">
         <v>0</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E12" t="s">
@@ -583,7 +728,7 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E13" t="s">
@@ -615,28 +760,34 @@
       <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -676,7 +827,7 @@
       <c r="C22" s="1">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E22" t="s">
@@ -687,7 +838,7 @@
       <c r="C23" s="1">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E23" t="s">
@@ -704,7 +855,7 @@
       <c r="C24" s="1">
         <v>12</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E24" t="s">
@@ -715,7 +866,7 @@
       <c r="C25" s="1">
         <v>13</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -756,92 +907,113 @@
       <c r="C32" s="1">
         <v>20</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C42" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>36</v>
       </c>
@@ -1086,82 +1258,89 @@
         <v>84</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C103" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C104" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C105" s="1">
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C106" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C107" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C108" s="1">
         <v>96</v>
       </c>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C109" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C110" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B111" s="4"/>
       <c r="C111" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="C112" s="1">
         <v>100</v>
       </c>
@@ -3699,6 +3878,93 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9AFE6D2-BA81-4052-8620-772E3222556C}">
+  <dimension ref="B2:S3"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="19" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>